<commit_message>
updated policy runs and calibration runs to update IPT and ART assumptions to match with HPV model, and differentiate incidence rates by policy
</commit_message>
<xml_diff>
--- a/KZN_south_africa/param_files/policy_eval_params/IPT_inititation_df.xlsx
+++ b/KZN_south_africa/param_files/policy_eval_params/IPT_inititation_df.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/param_files/policy_eval_params/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/KZN_south_africa/param_files/policy_eval_params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3428E7-902C-CF4E-B02E-B55312D01E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FE0C14-41F8-FD4A-8930-8B334A1AC703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="1160" windowWidth="14380" windowHeight="18060" activeTab="1" xr2:uid="{0D5B4E24-E2BC-434F-9926-FFC45EE0525A}"/>
+    <workbookView xWindow="19960" yWindow="1060" windowWidth="14380" windowHeight="18060" xr2:uid="{0D5B4E24-E2BC-434F-9926-FFC45EE0525A}"/>
   </bookViews>
   <sheets>
     <sheet name="warm_up" sheetId="1" r:id="rId1"/>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5232D7E8-72AD-0640-BDF6-FB7E1791E5B5}">
   <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="D101" s="1">
         <f>(D113-D100)/(A113-A100)</f>
-        <v>1.0769230769230769E-3</v>
+        <v>0</v>
       </c>
       <c r="E101" t="s">
         <v>8</v>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="D102" s="1">
         <f>$D$101+D101</f>
-        <v>2.1538461538461538E-3</v>
+        <v>0</v>
       </c>
       <c r="E102" t="s">
         <v>8</v>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="D103" s="1">
         <f t="shared" ref="D103:D112" si="3">$D$101+D102</f>
-        <v>3.2307692307692306E-3</v>
+        <v>0</v>
       </c>
       <c r="E103" t="s">
         <v>8</v>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D104" s="1">
         <f t="shared" si="3"/>
-        <v>4.3076923076923075E-3</v>
+        <v>0</v>
       </c>
       <c r="E104" t="s">
         <v>8</v>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="D105" s="1">
         <f t="shared" si="3"/>
-        <v>5.3846153846153844E-3</v>
+        <v>0</v>
       </c>
       <c r="E105" t="s">
         <v>8</v>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="D106" s="1">
         <f t="shared" si="3"/>
-        <v>6.4615384615384613E-3</v>
+        <v>0</v>
       </c>
       <c r="E106" t="s">
         <v>8</v>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="D107" s="1">
         <f t="shared" si="3"/>
-        <v>7.5384615384615382E-3</v>
+        <v>0</v>
       </c>
       <c r="E107" t="s">
         <v>8</v>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="D108" s="1">
         <f t="shared" si="3"/>
-        <v>8.615384615384615E-3</v>
+        <v>0</v>
       </c>
       <c r="E108" t="s">
         <v>8</v>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="D109" s="1">
         <f t="shared" si="3"/>
-        <v>9.692307692307691E-3</v>
+        <v>0</v>
       </c>
       <c r="E109" t="s">
         <v>8</v>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="D110" s="1">
         <f t="shared" si="3"/>
-        <v>1.0769230769230767E-2</v>
+        <v>0</v>
       </c>
       <c r="E110" t="s">
         <v>8</v>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D111" s="1">
         <f t="shared" si="3"/>
-        <v>1.1846153846153843E-2</v>
+        <v>0</v>
       </c>
       <c r="E111" t="s">
         <v>8</v>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="D112" s="1">
         <f t="shared" si="3"/>
-        <v>1.2923076923076919E-2</v>
+        <v>0</v>
       </c>
       <c r="E112" t="s">
         <v>8</v>
@@ -2394,7 +2394,7 @@
         <v>2</v>
       </c>
       <c r="D113" s="1">
-        <v>1.4E-2</v>
+        <v>0</v>
       </c>
       <c r="E113" t="s">
         <v>8</v>
@@ -2409,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BAE116D-E1C4-504C-B7CC-C6DC99B3E159}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2445,30 +2445,30 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>0.28999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4">
-        <v>0.7</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2476,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2493,15 +2493,15 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2510,12 +2510,12 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -2524,7 +2524,7 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <v>0.27</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2535,10 +2535,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D9">
-        <v>0.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2546,41 +2546,41 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11">
-        <v>1.4E-2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>1.4E-2</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2598,6 +2598,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D13">
+    <sortCondition ref="A2:A13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>